<commit_message>
Add final excel functions
</commit_message>
<xml_diff>
--- a/excel_processing/output.xlsx
+++ b/excel_processing/output.xlsx
@@ -1,9 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="1" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,36 +12,51 @@
     <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191028" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="&quot;£&quot;#,##0.00" numFmtId="164"/>
+    <numFmt formatCode="\£#,##0.00" numFmtId="164"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="10"/>
+      <color rgb="FF0563C1"/>
       <sz val="11"/>
       <u val="single"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -52,20 +68,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF4B183"/>
+        <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999755851924192"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFE699"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,30 +97,79 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="8"/>
+        <color rgb="FF4472C4"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle builtinId="8" name="*unknown*" xfId="6"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -150,7 +215,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -165,44 +229,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -229,15 +293,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -264,7 +327,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -276,482 +338,573 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="L1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L6" activeCellId="0" pane="topLeft" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="12" min="12" style="2" width="64.28515625"/>
-    <col customWidth="1" max="13" min="13" style="7" width="28.5703125"/>
+    <col customWidth="1" max="11" min="1" style="8" width="8.59"/>
+    <col customWidth="1" max="12" min="12" style="9" width="63.63"/>
+    <col customWidth="1" max="13" min="13" style="10" width="28.28"/>
+    <col customWidth="1" max="1025" min="14" style="8" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="1">
-      <c r="L1" s="3" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+      <c r="L1" s="11" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="11" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" r="2" s="4">
-      <c r="L2" s="2" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="15" r="2" s="12">
+      <c r="L2" s="9" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="M2" s="6" t="inlineStr">
+      <c r="M2" s="13" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="L3" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="3" s="14">
+      <c r="L3" s="9" t="inlineStr">
         <is>
           <t>of</t>
         </is>
       </c>
-      <c r="M3" s="7" t="inlineStr">
+      <c r="M3" s="10" t="inlineStr">
         <is>
           <t>the</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="L4" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="4" s="14">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>these</t>
         </is>
       </c>
-      <c r="M4" s="7" t="inlineStr">
+      <c r="M4" s="10" t="inlineStr">
         <is>
           <t>sheet</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="L5" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="5" s="14">
+      <c r="L5" s="9" t="inlineStr">
         <is>
           <t>cells</t>
         </is>
       </c>
-      <c r="M5" s="7" t="inlineStr">
+      <c r="M5" s="10" t="inlineStr">
         <is>
           <t>called</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="L6" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="6" s="14">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>are</t>
         </is>
       </c>
-      <c r="M6" s="7" t="inlineStr">
+      <c r="M6" s="10" t="inlineStr">
         <is>
           <t>"Summary"</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="L7" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="7" s="14">
+      <c r="L7" s="9" t="inlineStr">
         <is>
           <t>used</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="L8" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="8" s="14">
+      <c r="L8" s="9" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="L9" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="9" s="14">
+      <c r="L9" s="9" t="inlineStr">
         <is>
           <t>the</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="L10" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="10" s="14">
+      <c r="L10" s="9" t="inlineStr">
         <is>
           <t>macro</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet2">
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="M20" activeCellId="0" pane="topLeft" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="12" min="12" style="2" width="64.28515625"/>
-    <col customWidth="1" max="13" min="13" style="7" width="28.5703125"/>
+    <col customWidth="1" max="11" min="1" style="8" width="8.59"/>
+    <col customWidth="1" max="12" min="12" style="9" width="63.63"/>
+    <col customWidth="1" max="13" min="13" style="10" width="28.28"/>
+    <col customWidth="1" max="1025" min="14" style="8" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="1">
-      <c r="L1" s="3" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+      <c r="L1" s="11" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="11" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" r="2" s="4">
-      <c r="L2" s="8" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="13.8" r="2" s="12">
+      <c r="L2" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/lotsofsmallsteps</t>
         </is>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="13" t="inlineStr">
+        <is>
+          <t>33949.81</t>
+        </is>
+      </c>
+      <c r="N2" s="13" t="n">
         <v>33859.81</v>
       </c>
     </row>
-    <row r="3">
-      <c r="L3" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="3" s="14">
+      <c r="L3" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/alison-scott75</t>
         </is>
       </c>
-      <c r="M3" s="7" t="n">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>970</t>
+        </is>
+      </c>
+      <c r="N3" s="10" t="n">
         <v>938</v>
       </c>
     </row>
-    <row r="4">
-      <c r="L4" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="4" s="14">
+      <c r="L4" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/SPCPLive3</t>
         </is>
       </c>
-      <c r="M4" s="7" t="n">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>1510</t>
+        </is>
+      </c>
+      <c r="N4" s="10" t="n">
         <v>1330</v>
       </c>
     </row>
-    <row r="5">
-      <c r="L5" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="5" s="14">
+      <c r="L5" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/Ed-Jones4</t>
         </is>
       </c>
-      <c r="M5" s="7" t="n">
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>8901.69</t>
+        </is>
+      </c>
+      <c r="N5" s="10" t="n">
         <v>6362.13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="L6" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="6" s="14">
+      <c r="L6" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/Sarah-Wilson138</t>
         </is>
       </c>
-      <c r="M6" s="7" t="n">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>10010</t>
+        </is>
+      </c>
+      <c r="N6" s="10" t="n">
         <v>10010</v>
       </c>
     </row>
-    <row r="7">
-      <c r="L7" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="7" s="14">
+      <c r="L7" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/lexyeverest</t>
         </is>
       </c>
-      <c r="M7" s="7" t="n">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1370.19</t>
+        </is>
+      </c>
+      <c r="N7" s="10" t="n">
         <v>1315.19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L3 L7">
-    <cfRule dxfId="0" priority="5" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule dxfId="0" priority="4" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="3" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule dxfId="0" priority="3" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="4" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule dxfId="0" priority="2" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="5" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule dxfId="0" priority="1" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="6" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1"/>
-    <hyperlink ref="L4" r:id="rId2"/>
-    <hyperlink ref="L5" r:id="rId3"/>
+    <hyperlink display="https://www.justgiving.com/fundraising/alison-scott75" ref="L3" r:id="rId1"/>
+    <hyperlink display="https://www.justgiving.com/fundraising/SPCPLive3" ref="L4" r:id="rId2"/>
+    <hyperlink display="https://www.justgiving.com/fundraising/Ed-Jones4" ref="L5" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet3">
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="M1" activeCellId="0" pane="topLeft" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="12" min="12" style="2" width="64.28515625"/>
-    <col customWidth="1" max="13" min="13" style="7" width="28.5703125"/>
+    <col customWidth="1" max="11" min="1" style="8" width="8.59"/>
+    <col customWidth="1" max="12" min="12" style="9" width="63.63"/>
+    <col customWidth="1" max="13" min="13" style="10" width="28.28"/>
+    <col customWidth="1" max="1025" min="14" style="8" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="1">
-      <c r="L1" s="3" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="15" r="1" s="8">
+      <c r="L1" s="11" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="11" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" r="2" s="4">
-      <c r="L2" s="8" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="13.8" r="2" s="12">
+      <c r="L2" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/SWLondonMarathonTeam2018</t>
         </is>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="8" t="inlineStr">
+        <is>
+          <t>18854.15</t>
+        </is>
+      </c>
+      <c r="N2" s="13" t="n">
         <v>18129.15</v>
       </c>
     </row>
-    <row r="3">
-      <c r="L3" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="3" s="14">
+      <c r="L3" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/UCLAmyloidosisResearchFund</t>
         </is>
       </c>
-      <c r="M3" s="7" t="n">
+      <c r="M3" s="8" t="inlineStr">
+        <is>
+          <t>27264.88</t>
+        </is>
+      </c>
+      <c r="N3" s="10" t="n">
         <v>23309.88</v>
       </c>
     </row>
-    <row r="4">
-      <c r="L4" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="4" s="14">
+      <c r="L4" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/MaxsMissiontoMove</t>
         </is>
       </c>
-      <c r="M4" s="7" t="n">
+      <c r="M4" s="8" t="inlineStr">
+        <is>
+          <t>31165.76</t>
+        </is>
+      </c>
+      <c r="N4" s="10" t="n">
         <v>27811.38</v>
       </c>
     </row>
-    <row r="5">
-      <c r="L5" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="5" s="14">
+      <c r="L5" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/Michael-Jones09</t>
         </is>
       </c>
-      <c r="M5" s="7" t="n">
+      <c r="M5" s="8" t="inlineStr">
+        <is>
+          <t>1206</t>
+        </is>
+      </c>
+      <c r="N5" s="10" t="n">
         <v>1206</v>
       </c>
     </row>
-    <row r="6">
-      <c r="L6" s="8" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="6" s="14">
+      <c r="L6" s="15" t="inlineStr">
         <is>
           <t>https://www.justgiving.com/fundraising/chairmans125appeal</t>
         </is>
       </c>
-      <c r="M6" s="7" t="n">
+      <c r="M6" s="8" t="inlineStr">
+        <is>
+          <t>3815</t>
+        </is>
+      </c>
+      <c r="N6" s="10" t="n">
         <v>3165</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L6">
-    <cfRule dxfId="0" priority="1" type="containsBlanks">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" equalAverage="0" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(L2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1"/>
+    <hyperlink display="https://www.justgiving.com/fundraising/MaxsMissiontoMove" ref="L4" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>